<commit_message>
Updated Fall 19 Schedule, Updated next stop logic
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\GoogleActions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\GoogleActions\Spot-My-Blue-Bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A822A3-236D-4519-9DBE-ABC2EF75E291}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14C4F22-1D5F-44AA-B505-B739FBA6616F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="6" xr2:uid="{74405455-E426-47FC-B326-E014761D8B06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74405455-E426-47FC-B326-E014761D8B06}"/>
   </bookViews>
   <sheets>
     <sheet name="WSWeekOutbound" sheetId="1" r:id="rId1"/>
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3C9A48-CD7B-4773-B9CB-91265C4D164E}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2282,7 +2282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625B98FD-1A67-4708-8EF5-F789ABD0D047}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>